<commit_message>
add login - state streamlit
</commit_message>
<xml_diff>
--- a/drap_dashboard_pg.xlsx
+++ b/drap_dashboard_pg.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DATA\P&amp;G\my_project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BF00F5D-E790-4813-8604-93E748B68736}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECB96BE1-01EE-4871-AF60-DCBB57FF8D7E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28692" yWindow="-108" windowWidth="27852" windowHeight="16416" activeTab="1" xr2:uid="{81BED03A-7B47-40D2-AC37-CB6915E6066F}"/>
+    <workbookView xWindow="852" yWindow="-108" windowWidth="22296" windowHeight="13176" activeTab="3" xr2:uid="{81BED03A-7B47-40D2-AC37-CB6915E6066F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="DB_PG" sheetId="2" r:id="rId2"/>
     <sheet name="get_number_dashboard" sheetId="3" r:id="rId3"/>
+    <sheet name="drap_follow_login_state" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="560" uniqueCount="292">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="575" uniqueCount="304">
   <si>
     <t>inventory</t>
   </si>
@@ -944,6 +945,46 @@
   </si>
   <si>
     <t>Nhớ check lại sự tồn tại của các cột trước khi tính toán</t>
+  </si>
+  <si>
+    <t>components</t>
+  </si>
+  <si>
+    <t>header</t>
+  </si>
+  <si>
+    <t>render header title dashboard và thời gian</t>
+  </si>
+  <si>
+    <t>sidebar</t>
+  </si>
+  <si>
+    <t>pages</t>
+  </si>
+  <si>
+    <t>render trang login</t>
+  </si>
+  <si>
+    <t>profile</t>
+  </si>
+  <si>
+    <t>render profile user đang truy cập</t>
+  </si>
+  <si>
+    <t>render db, lấy data từ stage
+có thể thêm tùy chọn riêng cho sidebar của từng trang</t>
+  </si>
+  <si>
+    <t>Render sidebar, menu trang, button logout. Trả về trang được chọn cho pages
+Hiển thị các pages có trong chương trình và hiển thị theo role user nếu cần</t>
+  </si>
+  <si>
+    <t>main</t>
+  </si>
+  <si>
+    <t>Check xem user đã login chưa nếu chưa thì yc login
+Sau khi đã login thì chuyển sang render sidebar
+Sidebar sẽ trả về các trang tương ứng người dùng chọn. Sau đó sẽ chạy hàm rander_page đối với từng trang bằng câu lệnh if</t>
   </si>
 </sst>
 </file>
@@ -1012,7 +1053,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -1040,6 +1081,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1359,7 +1403,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A34" sqref="A34:B34"/>
+      <selection pane="bottomLeft" activeCell="C38" sqref="C38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1755,9 +1799,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5E52558-83A0-40C2-97FB-FA56B3A6B431}">
   <dimension ref="A1:I130"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A56" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B60" sqref="B60:E60"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A65" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E80" sqref="E80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3568,4 +3612,81 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B989CBF7-D183-40D0-A1F6-4A80D74D06FF}">
+  <dimension ref="A1:D7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D16" sqref="D13:D16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.6640625" customWidth="1"/>
+    <col min="4" max="4" width="65.88671875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>235</v>
+      </c>
+      <c r="B1" t="s">
+        <v>292</v>
+      </c>
+      <c r="C1" t="s">
+        <v>293</v>
+      </c>
+      <c r="D1" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="31.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C2" t="s">
+        <v>295</v>
+      </c>
+      <c r="D2" s="12" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B3" t="s">
+        <v>296</v>
+      </c>
+      <c r="C3" t="s">
+        <v>37</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C4" t="s">
+        <v>218</v>
+      </c>
+      <c r="D4" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C5" t="s">
+        <v>298</v>
+      </c>
+      <c r="D5" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>302</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>303</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
fix upload file moi dashboard khong refesh
</commit_message>
<xml_diff>
--- a/drap_dashboard_pg.xlsx
+++ b/drap_dashboard_pg.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DATA\P&amp;G\my_project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECB96BE1-01EE-4871-AF60-DCBB57FF8D7E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70A820B2-5507-4AC8-B4F0-C98B0DB9A042}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="852" yWindow="-108" windowWidth="22296" windowHeight="13176" activeTab="3" xr2:uid="{81BED03A-7B47-40D2-AC37-CB6915E6066F}"/>
+    <workbookView xWindow="852" yWindow="-108" windowWidth="22296" windowHeight="13176" activeTab="4" xr2:uid="{81BED03A-7B47-40D2-AC37-CB6915E6066F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="DB_PG" sheetId="2" r:id="rId2"/>
     <sheet name="get_number_dashboard" sheetId="3" r:id="rId3"/>
     <sheet name="drap_follow_login_state" sheetId="4" r:id="rId4"/>
+    <sheet name="note" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="575" uniqueCount="304">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="576" uniqueCount="305">
   <si>
     <t>inventory</t>
   </si>
@@ -985,6 +986,9 @@
     <t>Check xem user đã login chưa nếu chưa thì yc login
 Sau khi đã login thì chuyển sang render sidebar
 Sidebar sẽ trả về các trang tương ứng người dùng chọn. Sau đó sẽ chạy hàm rander_page đối với từng trang bằng câu lệnh if</t>
+  </si>
+  <si>
+    <t>Trong streamlit khi hàm on_change của một widget như st.button(), st.text_input(), st.slider(),  st.file_uploader().. Được kích hoạt, toàn bộ script Streamlit sẽ chạy lại từ đầu</t>
   </si>
 </sst>
 </file>
@@ -3618,8 +3622,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B989CBF7-D183-40D0-A1F6-4A80D74D06FF}">
   <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D16" sqref="D13:D16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3689,4 +3693,30 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B521056-CE0B-4BDC-B11A-8C3414C0DE1E}">
+  <dimension ref="A1:B1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="50.21875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A1" s="6">
+        <v>1</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>304</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>